<commit_message>
Subidos nuevos formatos de legalizacion y Pre-cuenta
</commit_message>
<xml_diff>
--- a/public/bd/Formato Solicitud y legalizacion de gastos.xlsx
+++ b/public/bd/Formato Solicitud y legalizacion de gastos.xlsx
@@ -173,32 +173,10 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>FORMATO DE LEGALIZACIÓN DE GASTOS</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-881-2013</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
+    <t xml:space="preserve">FORMATO DE LEGALIZACIÓN DE VIÁTICOS
+NOMBRE DEL PROYECTO/ INTERVENTORÍA
+NÚMERO Y AÑO DEL CONTRATO
 </t>
-    </r>
   </si>
 </sst>
 </file>
@@ -681,97 +659,97 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="165" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -799,20 +777,20 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -899,43 +877,44 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
+      <xdr:colOff>154781</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>107156</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1590040</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>8255</xdr:rowOff>
+      <xdr:colOff>1535906</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>511969</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Imagen 4">
+        <xdr:cNvPr id="6" name="Imagen 3" descr="H:\MANUAL COMUNICACIONES\MC\C&amp;M\Logos\7cm.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{61CFAC70-82BB-49D8-BE71-3A76F0F99520}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
+        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="142875" y="19050"/>
-          <a:ext cx="1447165" cy="1017905"/>
+          <a:off x="154781" y="107156"/>
+          <a:ext cx="1381125" cy="785813"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -950,96 +929,54 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1190624</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>226220</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1590040</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>8255</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1055686</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>35085</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagen 1">
+        <xdr:cNvPr id="3" name="Imagen 2" descr="C:\Users\Marcela.Barrios\AppData\Local\Microsoft\Windows\INetCache\Content.Outlook\54EIFNWQ\logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3F5F8055-5F93-41F6-B9CF-CF8A77DD95ED}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
+            <a:ext uri="{BEBA8EAE-BF5A-486C-A8C5-ECC9F3942E4B}">
+              <a14:imgProps xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a14:imgLayer r:embed="rId3">
+                  <a14:imgEffect>
+                    <a14:artisticPhotocopy/>
+                  </a14:imgEffect>
+                </a14:imgLayer>
+              </a14:imgProps>
+            </a:ext>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
+        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="142875" y="19050"/>
-          <a:ext cx="1447165" cy="1017905"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1590040</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>8255</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Imagen 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3F5F8055-5F93-41F6-B9CF-CF8A77DD95ED}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="142875" y="19050"/>
-          <a:ext cx="1447165" cy="1017905"/>
+          <a:off x="7798593" y="12680158"/>
+          <a:ext cx="3722687" cy="3856990"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1412,12 +1349,12 @@
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="57" t="s">
+      <c r="A5" s="77" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="57"/>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
+      <c r="B5" s="77"/>
+      <c r="C5" s="97"/>
+      <c r="D5" s="97"/>
       <c r="E5" s="6"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
@@ -1425,12 +1362,12 @@
       <c r="I5" s="8"/>
     </row>
     <row r="6" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="57" t="s">
+      <c r="A6" s="77" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="57"/>
-      <c r="C6" s="82"/>
-      <c r="D6" s="82"/>
+      <c r="B6" s="77"/>
+      <c r="C6" s="98"/>
+      <c r="D6" s="98"/>
       <c r="E6" s="10"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -1438,12 +1375,12 @@
       <c r="I6" s="8"/>
     </row>
     <row r="7" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="57" t="s">
+      <c r="A7" s="77" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="57"/>
-      <c r="C7" s="82"/>
-      <c r="D7" s="82"/>
+      <c r="B7" s="77"/>
+      <c r="C7" s="98"/>
+      <c r="D7" s="98"/>
       <c r="E7" s="10"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
@@ -1451,12 +1388,12 @@
       <c r="I7" s="8"/>
     </row>
     <row r="8" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="57" t="s">
+      <c r="A8" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="57"/>
-      <c r="C8" s="83"/>
-      <c r="D8" s="83"/>
+      <c r="B8" s="77"/>
+      <c r="C8" s="99"/>
+      <c r="D8" s="99"/>
       <c r="E8" s="11"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
@@ -1464,12 +1401,12 @@
       <c r="I8" s="8"/>
     </row>
     <row r="9" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="57" t="s">
+      <c r="A9" s="77" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="57"/>
-      <c r="C9" s="82"/>
-      <c r="D9" s="82"/>
+      <c r="B9" s="77"/>
+      <c r="C9" s="98"/>
+      <c r="D9" s="98"/>
       <c r="E9" s="11"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
@@ -1477,12 +1414,12 @@
       <c r="I9" s="8"/>
     </row>
     <row r="10" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="85" t="s">
+      <c r="A10" s="101" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="85"/>
-      <c r="C10" s="84"/>
-      <c r="D10" s="84"/>
+      <c r="B10" s="101"/>
+      <c r="C10" s="100"/>
+      <c r="D10" s="100"/>
       <c r="E10" s="11"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
@@ -1501,19 +1438,19 @@
       <c r="I11" s="15"/>
     </row>
     <row r="12" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="77" t="s">
+      <c r="A12" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="78"/>
-      <c r="C12" s="78"/>
-      <c r="D12" s="78"/>
+      <c r="B12" s="84"/>
+      <c r="C12" s="84"/>
+      <c r="D12" s="84"/>
       <c r="E12" s="11"/>
-      <c r="F12" s="78" t="s">
+      <c r="F12" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="G12" s="78"/>
-      <c r="H12" s="78"/>
-      <c r="I12" s="79"/>
+      <c r="G12" s="84"/>
+      <c r="H12" s="84"/>
+      <c r="I12" s="85"/>
     </row>
     <row r="13" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
@@ -1545,8 +1482,8 @@
     <row r="14" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="12"/>
       <c r="B14" s="12"/>
-      <c r="C14" s="86"/>
-      <c r="D14" s="86"/>
+      <c r="C14" s="57"/>
+      <c r="D14" s="57"/>
       <c r="E14" s="11"/>
       <c r="F14" s="13"/>
       <c r="G14" s="19"/>
@@ -1556,8 +1493,8 @@
     <row r="15" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="12"/>
       <c r="B15" s="12"/>
-      <c r="C15" s="86"/>
-      <c r="D15" s="86"/>
+      <c r="C15" s="57"/>
+      <c r="D15" s="57"/>
       <c r="E15" s="11"/>
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
@@ -1567,8 +1504,8 @@
     <row r="16" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="12"/>
       <c r="B16" s="12"/>
-      <c r="C16" s="86"/>
-      <c r="D16" s="86"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="57"/>
       <c r="E16" s="11"/>
       <c r="F16" s="17"/>
       <c r="G16" s="17"/>
@@ -1578,8 +1515,8 @@
     <row r="17" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="12"/>
       <c r="B17" s="12"/>
-      <c r="C17" s="86"/>
-      <c r="D17" s="86"/>
+      <c r="C17" s="57"/>
+      <c r="D17" s="57"/>
       <c r="E17" s="11"/>
       <c r="F17" s="17"/>
       <c r="G17" s="17"/>
@@ -1589,8 +1526,8 @@
     <row r="18" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="12"/>
       <c r="B18" s="12"/>
-      <c r="C18" s="86"/>
-      <c r="D18" s="86"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="57"/>
       <c r="E18" s="11"/>
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
@@ -1600,8 +1537,8 @@
     <row r="19" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="12"/>
       <c r="B19" s="12"/>
-      <c r="C19" s="86"/>
-      <c r="D19" s="86"/>
+      <c r="C19" s="57"/>
+      <c r="D19" s="57"/>
       <c r="E19" s="11"/>
       <c r="F19" s="17"/>
       <c r="G19" s="17"/>
@@ -1611,8 +1548,8 @@
     <row r="20" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="12"/>
       <c r="B20" s="12"/>
-      <c r="C20" s="86"/>
-      <c r="D20" s="86"/>
+      <c r="C20" s="57"/>
+      <c r="D20" s="57"/>
       <c r="E20" s="11"/>
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
@@ -1622,8 +1559,8 @@
     <row r="21" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="12"/>
       <c r="B21" s="12"/>
-      <c r="C21" s="86"/>
-      <c r="D21" s="86"/>
+      <c r="C21" s="57"/>
+      <c r="D21" s="57"/>
       <c r="E21" s="11"/>
       <c r="F21" s="17"/>
       <c r="G21" s="17"/>
@@ -1633,8 +1570,8 @@
     <row r="22" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="16"/>
       <c r="B22" s="17"/>
-      <c r="C22" s="87"/>
-      <c r="D22" s="86"/>
+      <c r="C22" s="58"/>
+      <c r="D22" s="57"/>
       <c r="E22" s="11"/>
       <c r="F22" s="17"/>
       <c r="G22" s="17"/>
@@ -1644,8 +1581,8 @@
     <row r="23" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="16"/>
       <c r="B23" s="17"/>
-      <c r="C23" s="87"/>
-      <c r="D23" s="86"/>
+      <c r="C23" s="58"/>
+      <c r="D23" s="57"/>
       <c r="E23" s="11"/>
       <c r="F23" s="17"/>
       <c r="G23" s="17"/>
@@ -1655,8 +1592,8 @@
     <row r="24" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="16"/>
       <c r="B24" s="17"/>
-      <c r="C24" s="87"/>
-      <c r="D24" s="86"/>
+      <c r="C24" s="58"/>
+      <c r="D24" s="57"/>
       <c r="E24" s="11"/>
       <c r="F24" s="17"/>
       <c r="G24" s="17"/>
@@ -1666,8 +1603,8 @@
     <row r="25" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="16"/>
       <c r="B25" s="17"/>
-      <c r="C25" s="87"/>
-      <c r="D25" s="86"/>
+      <c r="C25" s="58"/>
+      <c r="D25" s="57"/>
       <c r="E25" s="11"/>
       <c r="F25" s="17"/>
       <c r="G25" s="17"/>
@@ -1677,8 +1614,8 @@
     <row r="26" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="16"/>
       <c r="B26" s="17"/>
-      <c r="C26" s="87"/>
-      <c r="D26" s="86"/>
+      <c r="C26" s="58"/>
+      <c r="D26" s="57"/>
       <c r="E26" s="11"/>
       <c r="F26" s="17"/>
       <c r="G26" s="17"/>
@@ -1689,7 +1626,7 @@
       <c r="A27" s="20"/>
       <c r="B27" s="21"/>
       <c r="C27" s="22"/>
-      <c r="D27" s="86"/>
+      <c r="D27" s="57"/>
       <c r="E27" s="11"/>
       <c r="F27" s="23"/>
       <c r="G27" s="24"/>
@@ -1700,7 +1637,7 @@
       <c r="A28" s="20"/>
       <c r="B28" s="21"/>
       <c r="C28" s="22"/>
-      <c r="D28" s="86"/>
+      <c r="D28" s="57"/>
       <c r="E28" s="11"/>
       <c r="F28" s="23"/>
       <c r="G28" s="24"/>
@@ -1711,7 +1648,7 @@
       <c r="A29" s="20"/>
       <c r="B29" s="21"/>
       <c r="C29" s="22"/>
-      <c r="D29" s="86"/>
+      <c r="D29" s="57"/>
       <c r="E29" s="11"/>
       <c r="F29" s="23"/>
       <c r="G29" s="21"/>
@@ -1740,7 +1677,7 @@
       </c>
     </row>
     <row r="31" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A31" s="80" t="s">
+      <c r="A31" s="75" t="s">
         <v>10</v>
       </c>
       <c r="B31" s="76"/>
@@ -1761,11 +1698,11 @@
       </c>
     </row>
     <row r="32" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A32" s="74" t="s">
+      <c r="A32" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="B32" s="75"/>
-      <c r="C32" s="75"/>
+      <c r="B32" s="82"/>
+      <c r="C32" s="82"/>
       <c r="D32" s="28">
         <f>D31</f>
         <v>0</v>
@@ -1793,19 +1730,19 @@
       <c r="I33" s="33"/>
     </row>
     <row r="34" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="77" t="s">
+      <c r="A34" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="B34" s="78"/>
-      <c r="C34" s="78"/>
-      <c r="D34" s="78"/>
+      <c r="B34" s="84"/>
+      <c r="C34" s="84"/>
+      <c r="D34" s="84"/>
       <c r="E34" s="11"/>
-      <c r="F34" s="78" t="s">
+      <c r="F34" s="84" t="s">
         <v>15</v>
       </c>
-      <c r="G34" s="78"/>
-      <c r="H34" s="78"/>
-      <c r="I34" s="79"/>
+      <c r="G34" s="84"/>
+      <c r="H34" s="84"/>
+      <c r="I34" s="85"/>
     </row>
     <row r="35" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A35" s="16" t="s">
@@ -1931,7 +1868,7 @@
       <c r="I43" s="28"/>
     </row>
     <row r="44" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A44" s="80" t="s">
+      <c r="A44" s="75" t="s">
         <v>9</v>
       </c>
       <c r="B44" s="76"/>
@@ -1952,7 +1889,7 @@
       </c>
     </row>
     <row r="45" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A45" s="80" t="s">
+      <c r="A45" s="75" t="s">
         <v>10</v>
       </c>
       <c r="B45" s="76"/>
@@ -1973,7 +1910,7 @@
       </c>
     </row>
     <row r="46" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A46" s="80" t="s">
+      <c r="A46" s="75" t="s">
         <v>11</v>
       </c>
       <c r="B46" s="76"/>
@@ -2019,11 +1956,11 @@
       <c r="A49" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="B49" s="73">
+      <c r="B49" s="80">
         <f>D32+I30+D44</f>
         <v>0</v>
       </c>
-      <c r="C49" s="73"/>
+      <c r="C49" s="80"/>
       <c r="D49" s="10"/>
       <c r="E49" s="11"/>
       <c r="F49" s="10"/>
@@ -2035,11 +1972,11 @@
       <c r="A50" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="B50" s="73">
+      <c r="B50" s="80">
         <f>D32+I30+D44</f>
         <v>0</v>
       </c>
-      <c r="C50" s="73"/>
+      <c r="C50" s="80"/>
       <c r="D50" s="10"/>
       <c r="E50" s="11"/>
       <c r="F50" s="11"/>
@@ -2051,8 +1988,8 @@
       <c r="A51" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="B51" s="64"/>
-      <c r="C51" s="64"/>
+      <c r="B51" s="66"/>
+      <c r="C51" s="66"/>
       <c r="D51" s="10"/>
       <c r="E51" s="11"/>
       <c r="F51" s="11"/>
@@ -2071,14 +2008,14 @@
       <c r="H52" s="11"/>
       <c r="I52" s="15"/>
     </row>
-    <row r="53" spans="1:9" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A53" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="B53" s="65" t="s">
+      <c r="B53" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="C53" s="66"/>
+      <c r="C53" s="68"/>
       <c r="D53" s="10"/>
       <c r="E53" s="11"/>
       <c r="F53" s="11"/>
@@ -2091,10 +2028,10 @@
         <f>C6</f>
         <v>0</v>
       </c>
-      <c r="B54" s="67">
+      <c r="B54" s="69">
         <v>0</v>
       </c>
-      <c r="C54" s="68"/>
+      <c r="C54" s="70"/>
       <c r="D54" s="10"/>
       <c r="E54" s="11"/>
       <c r="F54" s="36"/>
@@ -2104,8 +2041,8 @@
     </row>
     <row r="55" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A55" s="40"/>
-      <c r="B55" s="67"/>
-      <c r="C55" s="68"/>
+      <c r="B55" s="69"/>
+      <c r="C55" s="70"/>
       <c r="D55" s="10"/>
       <c r="E55" s="11"/>
       <c r="F55" s="10"/>
@@ -2117,10 +2054,10 @@
       <c r="A56" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B56" s="69">
+      <c r="B56" s="71">
         <v>0</v>
       </c>
-      <c r="C56" s="70"/>
+      <c r="C56" s="72"/>
       <c r="D56" s="10"/>
       <c r="E56" s="11"/>
       <c r="F56" s="10"/>
@@ -2162,10 +2099,10 @@
       <c r="I59" s="44"/>
     </row>
     <row r="60" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A60" s="71" t="s">
+      <c r="A60" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="B60" s="72"/>
+      <c r="B60" s="74"/>
       <c r="C60" s="11"/>
       <c r="D60" s="11"/>
       <c r="E60" s="11"/>
@@ -2180,16 +2117,16 @@
       <c r="A61" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="B61" s="101"/>
-      <c r="C61" s="98"/>
+      <c r="B61" s="61"/>
+      <c r="C61" s="60"/>
       <c r="D61" s="11"/>
       <c r="E61" s="11"/>
       <c r="F61" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="G61" s="58"/>
-      <c r="H61" s="58"/>
-      <c r="I61" s="59"/>
+      <c r="G61" s="78"/>
+      <c r="H61" s="78"/>
+      <c r="I61" s="79"/>
     </row>
     <row r="62" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="47" t="s">
@@ -2202,9 +2139,9 @@
       <c r="F62" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="G62" s="99"/>
-      <c r="H62" s="99"/>
-      <c r="I62" s="100"/>
+      <c r="G62" s="86"/>
+      <c r="H62" s="86"/>
+      <c r="I62" s="87"/>
     </row>
     <row r="63" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A63" s="51"/>
@@ -2223,14 +2160,14 @@
       </c>
       <c r="B64" s="54"/>
       <c r="C64" s="11"/>
-      <c r="D64" s="60" t="s">
+      <c r="D64" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="E64" s="60"/>
-      <c r="F64" s="60"/>
-      <c r="G64" s="60"/>
-      <c r="H64" s="60"/>
-      <c r="I64" s="61"/>
+      <c r="E64" s="62"/>
+      <c r="F64" s="62"/>
+      <c r="G64" s="62"/>
+      <c r="H64" s="62"/>
+      <c r="I64" s="63"/>
     </row>
     <row r="65" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A65" s="39" t="s">
@@ -2238,12 +2175,12 @@
       </c>
       <c r="B65" s="21"/>
       <c r="C65" s="11"/>
-      <c r="D65" s="60"/>
-      <c r="E65" s="60"/>
-      <c r="F65" s="60"/>
-      <c r="G65" s="60"/>
-      <c r="H65" s="60"/>
-      <c r="I65" s="61"/>
+      <c r="D65" s="62"/>
+      <c r="E65" s="62"/>
+      <c r="F65" s="62"/>
+      <c r="G65" s="62"/>
+      <c r="H65" s="62"/>
+      <c r="I65" s="63"/>
     </row>
     <row r="66" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A66" s="39" t="s">
@@ -2251,12 +2188,12 @@
       </c>
       <c r="B66" s="21"/>
       <c r="C66" s="11"/>
-      <c r="D66" s="60"/>
-      <c r="E66" s="60"/>
-      <c r="F66" s="60"/>
-      <c r="G66" s="60"/>
-      <c r="H66" s="60"/>
-      <c r="I66" s="61"/>
+      <c r="D66" s="62"/>
+      <c r="E66" s="62"/>
+      <c r="F66" s="62"/>
+      <c r="G66" s="62"/>
+      <c r="H66" s="62"/>
+      <c r="I66" s="63"/>
     </row>
     <row r="67" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A67" s="39" t="s">
@@ -2264,25 +2201,25 @@
       </c>
       <c r="B67" s="21"/>
       <c r="C67" s="11"/>
-      <c r="D67" s="60"/>
-      <c r="E67" s="60"/>
-      <c r="F67" s="60"/>
-      <c r="G67" s="60"/>
-      <c r="H67" s="60"/>
-      <c r="I67" s="61"/>
+      <c r="D67" s="62"/>
+      <c r="E67" s="62"/>
+      <c r="F67" s="62"/>
+      <c r="G67" s="62"/>
+      <c r="H67" s="62"/>
+      <c r="I67" s="63"/>
     </row>
     <row r="68" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="B68" s="97"/>
+      <c r="B68" s="59"/>
       <c r="C68" s="56"/>
-      <c r="D68" s="62"/>
-      <c r="E68" s="62"/>
-      <c r="F68" s="62"/>
-      <c r="G68" s="62"/>
-      <c r="H68" s="62"/>
-      <c r="I68" s="63"/>
+      <c r="D68" s="64"/>
+      <c r="E68" s="64"/>
+      <c r="F68" s="64"/>
+      <c r="G68" s="64"/>
+      <c r="H68" s="64"/>
+      <c r="I68" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="39">
@@ -2302,17 +2239,22 @@
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="F46:H46"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="G61:I61"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="F34:I34"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A44:C44"/>
     <mergeCell ref="F44:H44"/>
     <mergeCell ref="A45:C45"/>
     <mergeCell ref="F45:H45"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="F46:H46"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="G61:I61"/>
     <mergeCell ref="D64:I68"/>
     <mergeCell ref="B51:C51"/>
     <mergeCell ref="B53:C53"/>
@@ -2320,11 +2262,6 @@
     <mergeCell ref="B55:C55"/>
     <mergeCell ref="B56:C56"/>
     <mergeCell ref="A60:B60"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="F34:I34"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2341,7 +2278,7 @@
   <dimension ref="A1:K68"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2405,12 +2342,12 @@
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="57" t="s">
+      <c r="A5" s="77" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="57"/>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
+      <c r="B5" s="77"/>
+      <c r="C5" s="97"/>
+      <c r="D5" s="97"/>
       <c r="E5" s="6"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
@@ -2418,12 +2355,12 @@
       <c r="I5" s="8"/>
     </row>
     <row r="6" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="57" t="s">
+      <c r="A6" s="77" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="57"/>
-      <c r="C6" s="82"/>
-      <c r="D6" s="82"/>
+      <c r="B6" s="77"/>
+      <c r="C6" s="98"/>
+      <c r="D6" s="98"/>
       <c r="E6" s="10"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -2431,12 +2368,12 @@
       <c r="I6" s="8"/>
     </row>
     <row r="7" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="57" t="s">
+      <c r="A7" s="77" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="57"/>
-      <c r="C7" s="82"/>
-      <c r="D7" s="82"/>
+      <c r="B7" s="77"/>
+      <c r="C7" s="98"/>
+      <c r="D7" s="98"/>
       <c r="E7" s="10"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
@@ -2444,12 +2381,12 @@
       <c r="I7" s="8"/>
     </row>
     <row r="8" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="57" t="s">
+      <c r="A8" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="57"/>
-      <c r="C8" s="83"/>
-      <c r="D8" s="83"/>
+      <c r="B8" s="77"/>
+      <c r="C8" s="99"/>
+      <c r="D8" s="99"/>
       <c r="E8" s="11"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
@@ -2457,12 +2394,12 @@
       <c r="I8" s="8"/>
     </row>
     <row r="9" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="57" t="s">
+      <c r="A9" s="77" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="57"/>
-      <c r="C9" s="82"/>
-      <c r="D9" s="82"/>
+      <c r="B9" s="77"/>
+      <c r="C9" s="98"/>
+      <c r="D9" s="98"/>
       <c r="E9" s="11"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
@@ -2470,12 +2407,12 @@
       <c r="I9" s="8"/>
     </row>
     <row r="10" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="85" t="s">
+      <c r="A10" s="101" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="85"/>
-      <c r="C10" s="84"/>
-      <c r="D10" s="84"/>
+      <c r="B10" s="101"/>
+      <c r="C10" s="100"/>
+      <c r="D10" s="100"/>
       <c r="E10" s="11"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
@@ -2494,19 +2431,19 @@
       <c r="I11" s="15"/>
     </row>
     <row r="12" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="77" t="s">
+      <c r="A12" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="78"/>
-      <c r="C12" s="78"/>
-      <c r="D12" s="78"/>
+      <c r="B12" s="84"/>
+      <c r="C12" s="84"/>
+      <c r="D12" s="84"/>
       <c r="E12" s="11"/>
-      <c r="F12" s="78" t="s">
+      <c r="F12" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="G12" s="78"/>
-      <c r="H12" s="78"/>
-      <c r="I12" s="79"/>
+      <c r="G12" s="84"/>
+      <c r="H12" s="84"/>
+      <c r="I12" s="85"/>
     </row>
     <row r="13" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
@@ -2538,8 +2475,8 @@
     <row r="14" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="12"/>
       <c r="B14" s="12"/>
-      <c r="C14" s="86"/>
-      <c r="D14" s="86"/>
+      <c r="C14" s="57"/>
+      <c r="D14" s="57"/>
       <c r="E14" s="11"/>
       <c r="F14" s="13"/>
       <c r="G14" s="19"/>
@@ -2549,8 +2486,8 @@
     <row r="15" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="12"/>
       <c r="B15" s="12"/>
-      <c r="C15" s="86"/>
-      <c r="D15" s="86"/>
+      <c r="C15" s="57"/>
+      <c r="D15" s="57"/>
       <c r="E15" s="11"/>
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
@@ -2560,8 +2497,8 @@
     <row r="16" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="12"/>
       <c r="B16" s="12"/>
-      <c r="C16" s="86"/>
-      <c r="D16" s="86"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="57"/>
       <c r="E16" s="11"/>
       <c r="F16" s="17"/>
       <c r="G16" s="17"/>
@@ -2571,8 +2508,8 @@
     <row r="17" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="12"/>
       <c r="B17" s="12"/>
-      <c r="C17" s="86"/>
-      <c r="D17" s="86"/>
+      <c r="C17" s="57"/>
+      <c r="D17" s="57"/>
       <c r="E17" s="11"/>
       <c r="F17" s="17"/>
       <c r="G17" s="17"/>
@@ -2582,8 +2519,8 @@
     <row r="18" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="12"/>
       <c r="B18" s="12"/>
-      <c r="C18" s="86"/>
-      <c r="D18" s="86"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="57"/>
       <c r="E18" s="11"/>
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
@@ -2593,8 +2530,8 @@
     <row r="19" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="12"/>
       <c r="B19" s="12"/>
-      <c r="C19" s="86"/>
-      <c r="D19" s="86"/>
+      <c r="C19" s="57"/>
+      <c r="D19" s="57"/>
       <c r="E19" s="11"/>
       <c r="F19" s="17"/>
       <c r="G19" s="17"/>
@@ -2604,8 +2541,8 @@
     <row r="20" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="12"/>
       <c r="B20" s="12"/>
-      <c r="C20" s="86"/>
-      <c r="D20" s="86"/>
+      <c r="C20" s="57"/>
+      <c r="D20" s="57"/>
       <c r="E20" s="11"/>
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
@@ -2615,8 +2552,8 @@
     <row r="21" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="12"/>
       <c r="B21" s="12"/>
-      <c r="C21" s="86"/>
-      <c r="D21" s="86"/>
+      <c r="C21" s="57"/>
+      <c r="D21" s="57"/>
       <c r="E21" s="11"/>
       <c r="F21" s="17"/>
       <c r="G21" s="17"/>
@@ -2626,8 +2563,8 @@
     <row r="22" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="16"/>
       <c r="B22" s="17"/>
-      <c r="C22" s="87"/>
-      <c r="D22" s="86"/>
+      <c r="C22" s="58"/>
+      <c r="D22" s="57"/>
       <c r="E22" s="11"/>
       <c r="F22" s="17"/>
       <c r="G22" s="17"/>
@@ -2637,8 +2574,8 @@
     <row r="23" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="16"/>
       <c r="B23" s="17"/>
-      <c r="C23" s="87"/>
-      <c r="D23" s="86"/>
+      <c r="C23" s="58"/>
+      <c r="D23" s="57"/>
       <c r="E23" s="11"/>
       <c r="F23" s="17"/>
       <c r="G23" s="17"/>
@@ -2648,8 +2585,8 @@
     <row r="24" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="16"/>
       <c r="B24" s="17"/>
-      <c r="C24" s="87"/>
-      <c r="D24" s="86"/>
+      <c r="C24" s="58"/>
+      <c r="D24" s="57"/>
       <c r="E24" s="11"/>
       <c r="F24" s="17"/>
       <c r="G24" s="17"/>
@@ -2659,8 +2596,8 @@
     <row r="25" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="16"/>
       <c r="B25" s="17"/>
-      <c r="C25" s="87"/>
-      <c r="D25" s="86"/>
+      <c r="C25" s="58"/>
+      <c r="D25" s="57"/>
       <c r="E25" s="11"/>
       <c r="F25" s="17"/>
       <c r="G25" s="17"/>
@@ -2670,8 +2607,8 @@
     <row r="26" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="16"/>
       <c r="B26" s="17"/>
-      <c r="C26" s="87"/>
-      <c r="D26" s="86"/>
+      <c r="C26" s="58"/>
+      <c r="D26" s="57"/>
       <c r="E26" s="11"/>
       <c r="F26" s="17"/>
       <c r="G26" s="17"/>
@@ -2682,7 +2619,7 @@
       <c r="A27" s="20"/>
       <c r="B27" s="21"/>
       <c r="C27" s="22"/>
-      <c r="D27" s="86"/>
+      <c r="D27" s="57"/>
       <c r="E27" s="11"/>
       <c r="F27" s="23"/>
       <c r="G27" s="24"/>
@@ -2693,7 +2630,7 @@
       <c r="A28" s="20"/>
       <c r="B28" s="21"/>
       <c r="C28" s="22"/>
-      <c r="D28" s="86"/>
+      <c r="D28" s="57"/>
       <c r="E28" s="11"/>
       <c r="F28" s="23"/>
       <c r="G28" s="24"/>
@@ -2704,7 +2641,7 @@
       <c r="A29" s="20"/>
       <c r="B29" s="21"/>
       <c r="C29" s="22"/>
-      <c r="D29" s="86"/>
+      <c r="D29" s="57"/>
       <c r="E29" s="11"/>
       <c r="F29" s="23"/>
       <c r="G29" s="21"/>
@@ -2733,7 +2670,7 @@
       </c>
     </row>
     <row r="31" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A31" s="80" t="s">
+      <c r="A31" s="75" t="s">
         <v>10</v>
       </c>
       <c r="B31" s="76"/>
@@ -2754,11 +2691,11 @@
       </c>
     </row>
     <row r="32" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A32" s="74" t="s">
+      <c r="A32" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="B32" s="75"/>
-      <c r="C32" s="75"/>
+      <c r="B32" s="82"/>
+      <c r="C32" s="82"/>
       <c r="D32" s="28">
         <f>D31</f>
         <v>0</v>
@@ -2786,19 +2723,19 @@
       <c r="I33" s="33"/>
     </row>
     <row r="34" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A34" s="77" t="s">
+      <c r="A34" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="B34" s="78"/>
-      <c r="C34" s="78"/>
-      <c r="D34" s="78"/>
+      <c r="B34" s="84"/>
+      <c r="C34" s="84"/>
+      <c r="D34" s="84"/>
       <c r="E34" s="11"/>
-      <c r="F34" s="78" t="s">
+      <c r="F34" s="84" t="s">
         <v>15</v>
       </c>
-      <c r="G34" s="78"/>
-      <c r="H34" s="78"/>
-      <c r="I34" s="79"/>
+      <c r="G34" s="84"/>
+      <c r="H34" s="84"/>
+      <c r="I34" s="85"/>
     </row>
     <row r="35" spans="1:9" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A35" s="16" t="s">
@@ -2916,7 +2853,7 @@
       <c r="I43" s="28"/>
     </row>
     <row r="44" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A44" s="80" t="s">
+      <c r="A44" s="75" t="s">
         <v>9</v>
       </c>
       <c r="B44" s="76"/>
@@ -2937,7 +2874,7 @@
       </c>
     </row>
     <row r="45" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A45" s="80" t="s">
+      <c r="A45" s="75" t="s">
         <v>10</v>
       </c>
       <c r="B45" s="76"/>
@@ -2958,7 +2895,7 @@
       </c>
     </row>
     <row r="46" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A46" s="80" t="s">
+      <c r="A46" s="75" t="s">
         <v>11</v>
       </c>
       <c r="B46" s="76"/>
@@ -3004,11 +2941,11 @@
       <c r="A49" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="B49" s="73">
+      <c r="B49" s="80">
         <f>D32+I30+D44</f>
         <v>0</v>
       </c>
-      <c r="C49" s="73"/>
+      <c r="C49" s="80"/>
       <c r="D49" s="10"/>
       <c r="E49" s="11"/>
       <c r="F49" s="10"/>
@@ -3020,11 +2957,11 @@
       <c r="A50" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="B50" s="73">
+      <c r="B50" s="80">
         <f>D32+I30+D44</f>
         <v>0</v>
       </c>
-      <c r="C50" s="73"/>
+      <c r="C50" s="80"/>
       <c r="D50" s="10"/>
       <c r="E50" s="11"/>
       <c r="F50" s="11"/>
@@ -3036,8 +2973,8 @@
       <c r="A51" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="B51" s="64"/>
-      <c r="C51" s="64"/>
+      <c r="B51" s="66"/>
+      <c r="C51" s="66"/>
       <c r="D51" s="10"/>
       <c r="E51" s="11"/>
       <c r="F51" s="11"/>
@@ -3062,10 +2999,10 @@
       <c r="A53" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="B53" s="65" t="s">
+      <c r="B53" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="C53" s="66"/>
+      <c r="C53" s="68"/>
       <c r="D53" s="10"/>
       <c r="E53" s="11"/>
       <c r="F53" s="11"/>
@@ -3078,10 +3015,10 @@
         <f>C6</f>
         <v>0</v>
       </c>
-      <c r="B54" s="67">
+      <c r="B54" s="69">
         <v>0</v>
       </c>
-      <c r="C54" s="68"/>
+      <c r="C54" s="70"/>
       <c r="D54" s="10"/>
       <c r="E54" s="11"/>
       <c r="F54" s="36"/>
@@ -3091,8 +3028,8 @@
     </row>
     <row r="55" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A55" s="40"/>
-      <c r="B55" s="67"/>
-      <c r="C55" s="68"/>
+      <c r="B55" s="69"/>
+      <c r="C55" s="70"/>
       <c r="D55" s="10"/>
       <c r="E55" s="11"/>
       <c r="F55" s="10"/>
@@ -3104,10 +3041,10 @@
       <c r="A56" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B56" s="69">
+      <c r="B56" s="71">
         <v>0</v>
       </c>
-      <c r="C56" s="70"/>
+      <c r="C56" s="72"/>
       <c r="D56" s="10"/>
       <c r="E56" s="11"/>
       <c r="F56" s="10"/>
@@ -3149,10 +3086,10 @@
       <c r="I59" s="44"/>
     </row>
     <row r="60" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A60" s="71" t="s">
+      <c r="A60" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="B60" s="72"/>
+      <c r="B60" s="74"/>
       <c r="C60" s="11"/>
       <c r="D60" s="11"/>
       <c r="E60" s="11"/>
@@ -3167,16 +3104,16 @@
       <c r="A61" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="B61" s="101"/>
-      <c r="C61" s="98"/>
+      <c r="B61" s="61"/>
+      <c r="C61" s="60"/>
       <c r="D61" s="11"/>
       <c r="E61" s="11"/>
       <c r="F61" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="G61" s="58"/>
-      <c r="H61" s="58"/>
-      <c r="I61" s="59"/>
+      <c r="G61" s="78"/>
+      <c r="H61" s="78"/>
+      <c r="I61" s="79"/>
     </row>
     <row r="62" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A62" s="47" t="s">
@@ -3189,9 +3126,9 @@
       <c r="F62" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="G62" s="99"/>
-      <c r="H62" s="99"/>
-      <c r="I62" s="100"/>
+      <c r="G62" s="86"/>
+      <c r="H62" s="86"/>
+      <c r="I62" s="87"/>
     </row>
     <row r="63" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A63" s="51"/>
@@ -3210,14 +3147,14 @@
       </c>
       <c r="B64" s="54"/>
       <c r="C64" s="11"/>
-      <c r="D64" s="60" t="s">
+      <c r="D64" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="E64" s="60"/>
-      <c r="F64" s="60"/>
-      <c r="G64" s="60"/>
-      <c r="H64" s="60"/>
-      <c r="I64" s="61"/>
+      <c r="E64" s="62"/>
+      <c r="F64" s="62"/>
+      <c r="G64" s="62"/>
+      <c r="H64" s="62"/>
+      <c r="I64" s="63"/>
     </row>
     <row r="65" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A65" s="39" t="s">
@@ -3225,12 +3162,12 @@
       </c>
       <c r="B65" s="21"/>
       <c r="C65" s="11"/>
-      <c r="D65" s="60"/>
-      <c r="E65" s="60"/>
-      <c r="F65" s="60"/>
-      <c r="G65" s="60"/>
-      <c r="H65" s="60"/>
-      <c r="I65" s="61"/>
+      <c r="D65" s="62"/>
+      <c r="E65" s="62"/>
+      <c r="F65" s="62"/>
+      <c r="G65" s="62"/>
+      <c r="H65" s="62"/>
+      <c r="I65" s="63"/>
     </row>
     <row r="66" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A66" s="39" t="s">
@@ -3238,12 +3175,12 @@
       </c>
       <c r="B66" s="21"/>
       <c r="C66" s="11"/>
-      <c r="D66" s="60"/>
-      <c r="E66" s="60"/>
-      <c r="F66" s="60"/>
-      <c r="G66" s="60"/>
-      <c r="H66" s="60"/>
-      <c r="I66" s="61"/>
+      <c r="D66" s="62"/>
+      <c r="E66" s="62"/>
+      <c r="F66" s="62"/>
+      <c r="G66" s="62"/>
+      <c r="H66" s="62"/>
+      <c r="I66" s="63"/>
     </row>
     <row r="67" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A67" s="39" t="s">
@@ -3251,25 +3188,25 @@
       </c>
       <c r="B67" s="21"/>
       <c r="C67" s="11"/>
-      <c r="D67" s="60"/>
-      <c r="E67" s="60"/>
-      <c r="F67" s="60"/>
-      <c r="G67" s="60"/>
-      <c r="H67" s="60"/>
-      <c r="I67" s="61"/>
+      <c r="D67" s="62"/>
+      <c r="E67" s="62"/>
+      <c r="F67" s="62"/>
+      <c r="G67" s="62"/>
+      <c r="H67" s="62"/>
+      <c r="I67" s="63"/>
     </row>
     <row r="68" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="B68" s="97"/>
+      <c r="B68" s="59"/>
       <c r="C68" s="56"/>
-      <c r="D68" s="62"/>
-      <c r="E68" s="62"/>
-      <c r="F68" s="62"/>
-      <c r="G68" s="62"/>
-      <c r="H68" s="62"/>
-      <c r="I68" s="63"/>
+      <c r="D68" s="64"/>
+      <c r="E68" s="64"/>
+      <c r="F68" s="64"/>
+      <c r="G68" s="64"/>
+      <c r="H68" s="64"/>
+      <c r="I68" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="39">
@@ -3304,14 +3241,14 @@
     <mergeCell ref="F30:H30"/>
     <mergeCell ref="A31:C31"/>
     <mergeCell ref="F31:H31"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="F45:H45"/>
     <mergeCell ref="A32:C32"/>
     <mergeCell ref="F32:H32"/>
     <mergeCell ref="A34:D34"/>
     <mergeCell ref="F34:I34"/>
     <mergeCell ref="A44:C44"/>
     <mergeCell ref="F44:H44"/>
-    <mergeCell ref="A45:C45"/>
-    <mergeCell ref="F45:H45"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Agregado FTP de UTKVD y NECH
</commit_message>
<xml_diff>
--- a/public/bd/Formato Solicitud y legalizacion de gastos.xlsx
+++ b/public/bd/Formato Solicitud y legalizacion de gastos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="60">
   <si>
     <t>TRANSPORTE</t>
   </si>
@@ -178,16 +178,68 @@
 NÚMERO Y AÑO DEL CONTRATO
 </t>
   </si>
+  <si>
+    <t>JAVIER IGNACIO CAICEDO SAMBONI</t>
+  </si>
+  <si>
+    <t>13/04/2018 - 18/04/2018</t>
+  </si>
+  <si>
+    <t>LETICIA</t>
+  </si>
+  <si>
+    <t>BASE AREA GAMMA</t>
+  </si>
+  <si>
+    <t>KM 11</t>
+  </si>
+  <si>
+    <t>KM 18</t>
+  </si>
+  <si>
+    <t>KM 6</t>
+  </si>
+  <si>
+    <t>EL VERGEL</t>
+  </si>
+  <si>
+    <t>ESTACIÓN GUARDA COSTA AMAZONAS</t>
+  </si>
+  <si>
+    <t>SAN SEBASTIAN</t>
+  </si>
+  <si>
+    <t>LA ESPERANZA</t>
+  </si>
+  <si>
+    <t>DESAYUNO</t>
+  </si>
+  <si>
+    <t>ALMUERZO</t>
+  </si>
+  <si>
+    <t>CENA</t>
+  </si>
+  <si>
+    <t>JAVIER CAICEDO</t>
+  </si>
+  <si>
+    <t>BANCOLOMBIA</t>
+  </si>
+  <si>
+    <t>AHORROS</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;\ * #,##0.00_);_(&quot;$&quot;\ * \(#,##0.00\);_(&quot;$&quot;\ * &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;\ * #,##0_);_(&quot;$&quot;\ * \(#,##0\);_(&quot;$&quot;\ * &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -258,6 +310,18 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -507,11 +571,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -673,6 +738,90 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -711,89 +860,21 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Moneda" xfId="2" builtinId="4"/>
     <cellStyle name="Moneda 2" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -835,7 +916,7 @@
         <xdr:cNvPr id="2" name="Imagen 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3F5F8055-5F93-41F6-B9CF-CF8A77DD95ED}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F5F8055-5F93-41F6-B9CF-CF8A77DD95ED}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -892,7 +973,7 @@
         <xdr:cNvPr id="6" name="Imagen 3" descr="H:\MANUAL COMUNICACIONES\MC\C&amp;M\Logos\7cm.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -945,7 +1026,7 @@
         <xdr:cNvPr id="3" name="Imagen 2" descr="C:\Users\Marcela.Barrios\AppData\Local\Microsoft\Windows\INetCache\Content.Outlook\54EIFNWQ\logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1303,39 +1384,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="67" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="90"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="69"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="91"/>
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="93"/>
+      <c r="A2" s="70"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="72"/>
     </row>
     <row r="3" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="94"/>
-      <c r="B3" s="95"/>
-      <c r="C3" s="95"/>
-      <c r="D3" s="95"/>
-      <c r="E3" s="95"/>
-      <c r="F3" s="95"/>
-      <c r="G3" s="95"/>
-      <c r="H3" s="95"/>
-      <c r="I3" s="96"/>
+      <c r="A3" s="73"/>
+      <c r="B3" s="74"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="75"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
@@ -1349,12 +1430,12 @@
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="77" t="s">
+      <c r="A5" s="63" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="77"/>
-      <c r="C5" s="97"/>
-      <c r="D5" s="97"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="81"/>
+      <c r="D5" s="81"/>
       <c r="E5" s="6"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
@@ -1362,12 +1443,12 @@
       <c r="I5" s="8"/>
     </row>
     <row r="6" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="77" t="s">
+      <c r="A6" s="63" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="77"/>
-      <c r="C6" s="98"/>
-      <c r="D6" s="98"/>
+      <c r="B6" s="63"/>
+      <c r="C6" s="82"/>
+      <c r="D6" s="82"/>
       <c r="E6" s="10"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -1375,12 +1456,12 @@
       <c r="I6" s="8"/>
     </row>
     <row r="7" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="77" t="s">
+      <c r="A7" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="77"/>
-      <c r="C7" s="98"/>
-      <c r="D7" s="98"/>
+      <c r="B7" s="63"/>
+      <c r="C7" s="82"/>
+      <c r="D7" s="82"/>
       <c r="E7" s="10"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
@@ -1388,12 +1469,12 @@
       <c r="I7" s="8"/>
     </row>
     <row r="8" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="77" t="s">
+      <c r="A8" s="63" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="77"/>
-      <c r="C8" s="99"/>
-      <c r="D8" s="99"/>
+      <c r="B8" s="63"/>
+      <c r="C8" s="83"/>
+      <c r="D8" s="83"/>
       <c r="E8" s="11"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
@@ -1401,12 +1482,12 @@
       <c r="I8" s="8"/>
     </row>
     <row r="9" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="77" t="s">
+      <c r="A9" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="77"/>
-      <c r="C9" s="98"/>
-      <c r="D9" s="98"/>
+      <c r="B9" s="63"/>
+      <c r="C9" s="82"/>
+      <c r="D9" s="82"/>
       <c r="E9" s="11"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
@@ -1414,12 +1495,12 @@
       <c r="I9" s="8"/>
     </row>
     <row r="10" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="101" t="s">
+      <c r="A10" s="85" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="101"/>
-      <c r="C10" s="100"/>
-      <c r="D10" s="100"/>
+      <c r="B10" s="85"/>
+      <c r="C10" s="84"/>
+      <c r="D10" s="84"/>
       <c r="E10" s="11"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
@@ -1438,19 +1519,19 @@
       <c r="I11" s="15"/>
     </row>
     <row r="12" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="83" t="s">
+      <c r="A12" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="84"/>
-      <c r="C12" s="84"/>
-      <c r="D12" s="84"/>
+      <c r="B12" s="77"/>
+      <c r="C12" s="77"/>
+      <c r="D12" s="77"/>
       <c r="E12" s="11"/>
-      <c r="F12" s="84" t="s">
+      <c r="F12" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="G12" s="84"/>
-      <c r="H12" s="84"/>
-      <c r="I12" s="85"/>
+      <c r="G12" s="77"/>
+      <c r="H12" s="77"/>
+      <c r="I12" s="78"/>
     </row>
     <row r="13" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
@@ -1666,53 +1747,53 @@
         <v>0</v>
       </c>
       <c r="E30" s="11"/>
-      <c r="F30" s="76" t="s">
+      <c r="F30" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="G30" s="76"/>
-      <c r="H30" s="76"/>
+      <c r="G30" s="79"/>
+      <c r="H30" s="79"/>
       <c r="I30" s="30">
         <f>SUM(I14:I29)</f>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A31" s="75" t="s">
+      <c r="A31" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="B31" s="76"/>
-      <c r="C31" s="76"/>
+      <c r="B31" s="79"/>
+      <c r="C31" s="79"/>
       <c r="D31" s="28">
         <f>D30</f>
         <v>0</v>
       </c>
       <c r="E31" s="11"/>
-      <c r="F31" s="76" t="s">
+      <c r="F31" s="79" t="s">
         <v>10</v>
       </c>
-      <c r="G31" s="76"/>
-      <c r="H31" s="76"/>
+      <c r="G31" s="79"/>
+      <c r="H31" s="79"/>
       <c r="I31" s="30">
         <f>I30</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A32" s="81" t="s">
+      <c r="A32" s="88" t="s">
         <v>11</v>
       </c>
-      <c r="B32" s="82"/>
-      <c r="C32" s="82"/>
+      <c r="B32" s="89"/>
+      <c r="C32" s="89"/>
       <c r="D32" s="28">
         <f>D31</f>
         <v>0</v>
       </c>
       <c r="E32" s="11"/>
-      <c r="F32" s="76" t="s">
+      <c r="F32" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="G32" s="76"/>
-      <c r="H32" s="76"/>
+      <c r="G32" s="79"/>
+      <c r="H32" s="79"/>
       <c r="I32" s="30">
         <f>I30</f>
         <v>0</v>
@@ -1730,19 +1811,19 @@
       <c r="I33" s="33"/>
     </row>
     <row r="34" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="83" t="s">
+      <c r="A34" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="B34" s="84"/>
-      <c r="C34" s="84"/>
-      <c r="D34" s="84"/>
+      <c r="B34" s="77"/>
+      <c r="C34" s="77"/>
+      <c r="D34" s="77"/>
       <c r="E34" s="11"/>
-      <c r="F34" s="84" t="s">
+      <c r="F34" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="G34" s="84"/>
-      <c r="H34" s="84"/>
-      <c r="I34" s="85"/>
+      <c r="G34" s="77"/>
+      <c r="H34" s="77"/>
+      <c r="I34" s="78"/>
     </row>
     <row r="35" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A35" s="16" t="s">
@@ -1868,63 +1949,63 @@
       <c r="I43" s="28"/>
     </row>
     <row r="44" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A44" s="75" t="s">
+      <c r="A44" s="80" t="s">
         <v>9</v>
       </c>
-      <c r="B44" s="76"/>
-      <c r="C44" s="76"/>
+      <c r="B44" s="79"/>
+      <c r="C44" s="79"/>
       <c r="D44" s="28">
         <f>SUM(D36:D43)</f>
         <v>0</v>
       </c>
       <c r="E44" s="11"/>
-      <c r="F44" s="76" t="s">
+      <c r="F44" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="G44" s="76"/>
-      <c r="H44" s="76"/>
+      <c r="G44" s="79"/>
+      <c r="H44" s="79"/>
       <c r="I44" s="25">
         <f>SUM(I36:I43)</f>
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A45" s="75" t="s">
+      <c r="A45" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="B45" s="76"/>
-      <c r="C45" s="76"/>
+      <c r="B45" s="79"/>
+      <c r="C45" s="79"/>
       <c r="D45" s="28">
         <f>D44</f>
         <v>0</v>
       </c>
       <c r="E45" s="11"/>
-      <c r="F45" s="76" t="s">
+      <c r="F45" s="79" t="s">
         <v>10</v>
       </c>
-      <c r="G45" s="76"/>
-      <c r="H45" s="76"/>
+      <c r="G45" s="79"/>
+      <c r="H45" s="79"/>
       <c r="I45" s="25">
         <f>I44</f>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A46" s="75" t="s">
+      <c r="A46" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="B46" s="76"/>
-      <c r="C46" s="76"/>
+      <c r="B46" s="79"/>
+      <c r="C46" s="79"/>
       <c r="D46" s="28">
         <f>D44</f>
         <v>0</v>
       </c>
       <c r="E46" s="11"/>
-      <c r="F46" s="76" t="s">
+      <c r="F46" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="G46" s="76"/>
-      <c r="H46" s="76"/>
+      <c r="G46" s="79"/>
+      <c r="H46" s="79"/>
       <c r="I46" s="25">
         <f>I44</f>
         <v>0</v>
@@ -1956,11 +2037,11 @@
       <c r="A49" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="B49" s="80">
+      <c r="B49" s="66">
         <f>D32+I30+D44</f>
         <v>0</v>
       </c>
-      <c r="C49" s="80"/>
+      <c r="C49" s="66"/>
       <c r="D49" s="10"/>
       <c r="E49" s="11"/>
       <c r="F49" s="10"/>
@@ -1972,11 +2053,11 @@
       <c r="A50" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="B50" s="80">
+      <c r="B50" s="66">
         <f>D32+I30+D44</f>
         <v>0</v>
       </c>
-      <c r="C50" s="80"/>
+      <c r="C50" s="66"/>
       <c r="D50" s="10"/>
       <c r="E50" s="11"/>
       <c r="F50" s="11"/>
@@ -1988,8 +2069,8 @@
       <c r="A51" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="B51" s="66"/>
-      <c r="C51" s="66"/>
+      <c r="B51" s="94"/>
+      <c r="C51" s="94"/>
       <c r="D51" s="10"/>
       <c r="E51" s="11"/>
       <c r="F51" s="11"/>
@@ -2012,10 +2093,10 @@
       <c r="A53" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="B53" s="67" t="s">
+      <c r="B53" s="95" t="s">
         <v>18</v>
       </c>
-      <c r="C53" s="68"/>
+      <c r="C53" s="96"/>
       <c r="D53" s="10"/>
       <c r="E53" s="11"/>
       <c r="F53" s="11"/>
@@ -2028,10 +2109,10 @@
         <f>C6</f>
         <v>0</v>
       </c>
-      <c r="B54" s="69">
+      <c r="B54" s="97">
         <v>0</v>
       </c>
-      <c r="C54" s="70"/>
+      <c r="C54" s="98"/>
       <c r="D54" s="10"/>
       <c r="E54" s="11"/>
       <c r="F54" s="36"/>
@@ -2041,8 +2122,8 @@
     </row>
     <row r="55" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A55" s="40"/>
-      <c r="B55" s="69"/>
-      <c r="C55" s="70"/>
+      <c r="B55" s="97"/>
+      <c r="C55" s="98"/>
       <c r="D55" s="10"/>
       <c r="E55" s="11"/>
       <c r="F55" s="10"/>
@@ -2054,10 +2135,10 @@
       <c r="A56" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B56" s="71">
+      <c r="B56" s="99">
         <v>0</v>
       </c>
-      <c r="C56" s="72"/>
+      <c r="C56" s="100"/>
       <c r="D56" s="10"/>
       <c r="E56" s="11"/>
       <c r="F56" s="10"/>
@@ -2099,10 +2180,10 @@
       <c r="I59" s="44"/>
     </row>
     <row r="60" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A60" s="73" t="s">
+      <c r="A60" s="101" t="s">
         <v>20</v>
       </c>
-      <c r="B60" s="74"/>
+      <c r="B60" s="102"/>
       <c r="C60" s="11"/>
       <c r="D60" s="11"/>
       <c r="E60" s="11"/>
@@ -2124,9 +2205,9 @@
       <c r="F61" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="G61" s="78"/>
-      <c r="H61" s="78"/>
-      <c r="I61" s="79"/>
+      <c r="G61" s="86"/>
+      <c r="H61" s="86"/>
+      <c r="I61" s="87"/>
     </row>
     <row r="62" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="47" t="s">
@@ -2139,9 +2220,9 @@
       <c r="F62" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="G62" s="86"/>
-      <c r="H62" s="86"/>
-      <c r="I62" s="87"/>
+      <c r="G62" s="64"/>
+      <c r="H62" s="64"/>
+      <c r="I62" s="65"/>
     </row>
     <row r="63" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A63" s="51"/>
@@ -2160,14 +2241,14 @@
       </c>
       <c r="B64" s="54"/>
       <c r="C64" s="11"/>
-      <c r="D64" s="62" t="s">
+      <c r="D64" s="90" t="s">
         <v>25</v>
       </c>
-      <c r="E64" s="62"/>
-      <c r="F64" s="62"/>
-      <c r="G64" s="62"/>
-      <c r="H64" s="62"/>
-      <c r="I64" s="63"/>
+      <c r="E64" s="90"/>
+      <c r="F64" s="90"/>
+      <c r="G64" s="90"/>
+      <c r="H64" s="90"/>
+      <c r="I64" s="91"/>
     </row>
     <row r="65" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A65" s="39" t="s">
@@ -2175,12 +2256,12 @@
       </c>
       <c r="B65" s="21"/>
       <c r="C65" s="11"/>
-      <c r="D65" s="62"/>
-      <c r="E65" s="62"/>
-      <c r="F65" s="62"/>
-      <c r="G65" s="62"/>
-      <c r="H65" s="62"/>
-      <c r="I65" s="63"/>
+      <c r="D65" s="90"/>
+      <c r="E65" s="90"/>
+      <c r="F65" s="90"/>
+      <c r="G65" s="90"/>
+      <c r="H65" s="90"/>
+      <c r="I65" s="91"/>
     </row>
     <row r="66" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A66" s="39" t="s">
@@ -2188,12 +2269,12 @@
       </c>
       <c r="B66" s="21"/>
       <c r="C66" s="11"/>
-      <c r="D66" s="62"/>
-      <c r="E66" s="62"/>
-      <c r="F66" s="62"/>
-      <c r="G66" s="62"/>
-      <c r="H66" s="62"/>
-      <c r="I66" s="63"/>
+      <c r="D66" s="90"/>
+      <c r="E66" s="90"/>
+      <c r="F66" s="90"/>
+      <c r="G66" s="90"/>
+      <c r="H66" s="90"/>
+      <c r="I66" s="91"/>
     </row>
     <row r="67" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A67" s="39" t="s">
@@ -2201,12 +2282,12 @@
       </c>
       <c r="B67" s="21"/>
       <c r="C67" s="11"/>
-      <c r="D67" s="62"/>
-      <c r="E67" s="62"/>
-      <c r="F67" s="62"/>
-      <c r="G67" s="62"/>
-      <c r="H67" s="62"/>
-      <c r="I67" s="63"/>
+      <c r="D67" s="90"/>
+      <c r="E67" s="90"/>
+      <c r="F67" s="90"/>
+      <c r="G67" s="90"/>
+      <c r="H67" s="90"/>
+      <c r="I67" s="91"/>
     </row>
     <row r="68" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68" s="55" t="s">
@@ -2214,15 +2295,38 @@
       </c>
       <c r="B68" s="59"/>
       <c r="C68" s="56"/>
-      <c r="D68" s="64"/>
-      <c r="E68" s="64"/>
-      <c r="F68" s="64"/>
-      <c r="G68" s="64"/>
-      <c r="H68" s="64"/>
-      <c r="I68" s="65"/>
+      <c r="D68" s="92"/>
+      <c r="E68" s="92"/>
+      <c r="F68" s="92"/>
+      <c r="G68" s="92"/>
+      <c r="H68" s="92"/>
+      <c r="I68" s="93"/>
     </row>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="D64:I68"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="F46:H46"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="G61:I61"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="F44:H44"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="F45:H45"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="G62:I62"/>
     <mergeCell ref="B49:C49"/>
@@ -2239,29 +2343,6 @@
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="F46:H46"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="G61:I61"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="F44:H44"/>
-    <mergeCell ref="A45:C45"/>
-    <mergeCell ref="F45:H45"/>
-    <mergeCell ref="D64:I68"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="A60:B60"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2277,15 +2358,15 @@
   </sheetPr>
   <dimension ref="A1:K68"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A47" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.85546875" style="4" customWidth="1"/>
     <col min="2" max="2" width="22.5703125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.5703125" style="4" customWidth="1"/>
     <col min="6" max="6" width="26.5703125" style="4" customWidth="1"/>
@@ -2296,39 +2377,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="67" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="90"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="69"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="91"/>
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="93"/>
+      <c r="A2" s="70"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="72"/>
     </row>
     <row r="3" spans="1:9" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="94"/>
-      <c r="B3" s="95"/>
-      <c r="C3" s="95"/>
-      <c r="D3" s="95"/>
-      <c r="E3" s="95"/>
-      <c r="F3" s="95"/>
-      <c r="G3" s="95"/>
-      <c r="H3" s="95"/>
-      <c r="I3" s="96"/>
+      <c r="A3" s="73"/>
+      <c r="B3" s="74"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="75"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
@@ -2342,12 +2423,14 @@
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="77" t="s">
+      <c r="A5" s="63" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="77"/>
-      <c r="C5" s="97"/>
-      <c r="D5" s="97"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="103">
+        <v>43202</v>
+      </c>
+      <c r="D5" s="104"/>
       <c r="E5" s="6"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
@@ -2355,12 +2438,14 @@
       <c r="I5" s="8"/>
     </row>
     <row r="6" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="77" t="s">
+      <c r="A6" s="63" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="77"/>
-      <c r="C6" s="98"/>
-      <c r="D6" s="98"/>
+      <c r="B6" s="63"/>
+      <c r="C6" s="82" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="82"/>
       <c r="E6" s="10"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -2368,12 +2453,14 @@
       <c r="I6" s="8"/>
     </row>
     <row r="7" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="77" t="s">
+      <c r="A7" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="B7" s="77"/>
-      <c r="C7" s="98"/>
-      <c r="D7" s="98"/>
+      <c r="B7" s="63"/>
+      <c r="C7" s="82">
+        <v>83040450</v>
+      </c>
+      <c r="D7" s="82"/>
       <c r="E7" s="10"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
@@ -2381,12 +2468,14 @@
       <c r="I7" s="8"/>
     </row>
     <row r="8" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="77" t="s">
+      <c r="A8" s="63" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="77"/>
-      <c r="C8" s="99"/>
-      <c r="D8" s="99"/>
+      <c r="B8" s="63"/>
+      <c r="C8" s="83" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="83"/>
       <c r="E8" s="11"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
@@ -2394,12 +2483,14 @@
       <c r="I8" s="8"/>
     </row>
     <row r="9" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="77" t="s">
+      <c r="A9" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="77"/>
-      <c r="C9" s="98"/>
-      <c r="D9" s="98"/>
+      <c r="B9" s="63"/>
+      <c r="C9" s="82" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="82"/>
       <c r="E9" s="11"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
@@ -2407,12 +2498,12 @@
       <c r="I9" s="8"/>
     </row>
     <row r="10" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="101" t="s">
+      <c r="A10" s="85" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="101"/>
-      <c r="C10" s="100"/>
-      <c r="D10" s="100"/>
+      <c r="B10" s="85"/>
+      <c r="C10" s="84"/>
+      <c r="D10" s="84"/>
       <c r="E10" s="11"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
@@ -2431,19 +2522,19 @@
       <c r="I11" s="15"/>
     </row>
     <row r="12" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="83" t="s">
+      <c r="A12" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="84"/>
-      <c r="C12" s="84"/>
-      <c r="D12" s="84"/>
+      <c r="B12" s="77"/>
+      <c r="C12" s="77"/>
+      <c r="D12" s="77"/>
       <c r="E12" s="11"/>
-      <c r="F12" s="84" t="s">
+      <c r="F12" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="G12" s="84"/>
-      <c r="H12" s="84"/>
-      <c r="I12" s="85"/>
+      <c r="G12" s="77"/>
+      <c r="H12" s="77"/>
+      <c r="I12" s="78"/>
     </row>
     <row r="13" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
@@ -2473,21 +2564,45 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="57"/>
+      <c r="A14" s="105" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="62">
+        <v>1</v>
+      </c>
+      <c r="C14" s="106">
+        <v>90000</v>
+      </c>
+      <c r="D14" s="106">
+        <v>90000</v>
+      </c>
       <c r="E14" s="11"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="28"/>
+      <c r="F14" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" s="19">
+        <v>7</v>
+      </c>
+      <c r="H14" s="28">
+        <v>60000</v>
+      </c>
+      <c r="I14" s="28">
+        <v>420000</v>
+      </c>
     </row>
     <row r="15" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="57"/>
-      <c r="D15" s="57"/>
+      <c r="A15" s="105" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="62">
+        <v>1</v>
+      </c>
+      <c r="C15" s="106">
+        <v>90000</v>
+      </c>
+      <c r="D15" s="106">
+        <v>90000</v>
+      </c>
       <c r="E15" s="11"/>
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
@@ -2495,10 +2610,18 @@
       <c r="I15" s="28"/>
     </row>
     <row r="16" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="57"/>
-      <c r="D16" s="57"/>
+      <c r="A16" s="105" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="62">
+        <v>1</v>
+      </c>
+      <c r="C16" s="106">
+        <v>90000</v>
+      </c>
+      <c r="D16" s="106">
+        <v>90000</v>
+      </c>
       <c r="E16" s="11"/>
       <c r="F16" s="17"/>
       <c r="G16" s="17"/>
@@ -2506,10 +2629,18 @@
       <c r="I16" s="28"/>
     </row>
     <row r="17" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="57"/>
-      <c r="D17" s="57"/>
+      <c r="A17" s="105" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="62">
+        <v>1</v>
+      </c>
+      <c r="C17" s="106">
+        <v>90000</v>
+      </c>
+      <c r="D17" s="106">
+        <v>90000</v>
+      </c>
       <c r="E17" s="11"/>
       <c r="F17" s="17"/>
       <c r="G17" s="17"/>
@@ -2517,10 +2648,18 @@
       <c r="I17" s="28"/>
     </row>
     <row r="18" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="57"/>
-      <c r="D18" s="57"/>
+      <c r="A18" s="105" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="62">
+        <v>1</v>
+      </c>
+      <c r="C18" s="106">
+        <v>90000</v>
+      </c>
+      <c r="D18" s="106">
+        <v>90000</v>
+      </c>
       <c r="E18" s="11"/>
       <c r="F18" s="17"/>
       <c r="G18" s="17"/>
@@ -2528,10 +2667,18 @@
       <c r="I18" s="28"/>
     </row>
     <row r="19" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="57"/>
-      <c r="D19" s="57"/>
+      <c r="A19" s="105" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="62">
+        <v>1</v>
+      </c>
+      <c r="C19" s="106">
+        <v>90000</v>
+      </c>
+      <c r="D19" s="106">
+        <v>90000</v>
+      </c>
       <c r="E19" s="11"/>
       <c r="F19" s="17"/>
       <c r="G19" s="17"/>
@@ -2539,10 +2686,18 @@
       <c r="I19" s="28"/>
     </row>
     <row r="20" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="57"/>
-      <c r="D20" s="57"/>
+      <c r="A20" s="105" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="62">
+        <v>1</v>
+      </c>
+      <c r="C20" s="106">
+        <v>90000</v>
+      </c>
+      <c r="D20" s="106">
+        <v>90000</v>
+      </c>
       <c r="E20" s="11"/>
       <c r="F20" s="17"/>
       <c r="G20" s="17"/>
@@ -2550,10 +2705,18 @@
       <c r="I20" s="28"/>
     </row>
     <row r="21" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="57"/>
-      <c r="D21" s="57"/>
+      <c r="A21" s="105" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="62">
+        <v>1</v>
+      </c>
+      <c r="C21" s="106">
+        <v>90000</v>
+      </c>
+      <c r="D21" s="106">
+        <v>90000</v>
+      </c>
       <c r="E21" s="11"/>
       <c r="F21" s="17"/>
       <c r="G21" s="17"/>
@@ -2561,10 +2724,18 @@
       <c r="I21" s="28"/>
     </row>
     <row r="22" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="16"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="58"/>
-      <c r="D22" s="57"/>
+      <c r="A22" s="105" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="17">
+        <v>1</v>
+      </c>
+      <c r="C22" s="106">
+        <v>90000</v>
+      </c>
+      <c r="D22" s="106">
+        <v>90000</v>
+      </c>
       <c r="E22" s="11"/>
       <c r="F22" s="17"/>
       <c r="G22" s="17"/>
@@ -2572,10 +2743,18 @@
       <c r="I22" s="28"/>
     </row>
     <row r="23" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="16"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="58"/>
-      <c r="D23" s="57"/>
+      <c r="A23" s="105" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="17">
+        <v>1</v>
+      </c>
+      <c r="C23" s="106">
+        <v>90000</v>
+      </c>
+      <c r="D23" s="106">
+        <v>90000</v>
+      </c>
       <c r="E23" s="11"/>
       <c r="F23" s="17"/>
       <c r="G23" s="17"/>
@@ -2583,10 +2762,18 @@
       <c r="I23" s="28"/>
     </row>
     <row r="24" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A24" s="16"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="58"/>
-      <c r="D24" s="57"/>
+      <c r="A24" s="105" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="17">
+        <v>1</v>
+      </c>
+      <c r="C24" s="106">
+        <v>90000</v>
+      </c>
+      <c r="D24" s="106">
+        <v>90000</v>
+      </c>
       <c r="E24" s="11"/>
       <c r="F24" s="17"/>
       <c r="G24" s="17"/>
@@ -2656,59 +2843,59 @@
       <c r="C30" s="29"/>
       <c r="D30" s="28">
         <f>SUM(D13:D29)</f>
-        <v>0</v>
+        <v>990000</v>
       </c>
       <c r="E30" s="11"/>
-      <c r="F30" s="76" t="s">
+      <c r="F30" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="G30" s="76"/>
-      <c r="H30" s="76"/>
+      <c r="G30" s="79"/>
+      <c r="H30" s="79"/>
       <c r="I30" s="30">
         <f>SUM(I14:I29)</f>
-        <v>0</v>
+        <v>420000</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A31" s="75" t="s">
+      <c r="A31" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="B31" s="76"/>
-      <c r="C31" s="76"/>
+      <c r="B31" s="79"/>
+      <c r="C31" s="79"/>
       <c r="D31" s="28">
         <f>D30</f>
-        <v>0</v>
+        <v>990000</v>
       </c>
       <c r="E31" s="11"/>
-      <c r="F31" s="76" t="s">
+      <c r="F31" s="79" t="s">
         <v>10</v>
       </c>
-      <c r="G31" s="76"/>
-      <c r="H31" s="76"/>
+      <c r="G31" s="79"/>
+      <c r="H31" s="79"/>
       <c r="I31" s="30">
         <f>I30</f>
-        <v>0</v>
+        <v>420000</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A32" s="81" t="s">
+      <c r="A32" s="88" t="s">
         <v>11</v>
       </c>
-      <c r="B32" s="82"/>
-      <c r="C32" s="82"/>
+      <c r="B32" s="89"/>
+      <c r="C32" s="89"/>
       <c r="D32" s="28">
         <f>D31</f>
-        <v>0</v>
+        <v>990000</v>
       </c>
       <c r="E32" s="11"/>
-      <c r="F32" s="76" t="s">
+      <c r="F32" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="G32" s="76"/>
-      <c r="H32" s="76"/>
+      <c r="G32" s="79"/>
+      <c r="H32" s="79"/>
       <c r="I32" s="30">
         <f>I30</f>
-        <v>0</v>
+        <v>420000</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
@@ -2723,19 +2910,19 @@
       <c r="I33" s="33"/>
     </row>
     <row r="34" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A34" s="83" t="s">
+      <c r="A34" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="B34" s="84"/>
-      <c r="C34" s="84"/>
-      <c r="D34" s="84"/>
+      <c r="B34" s="77"/>
+      <c r="C34" s="77"/>
+      <c r="D34" s="77"/>
       <c r="E34" s="11"/>
-      <c r="F34" s="84" t="s">
+      <c r="F34" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="G34" s="84"/>
-      <c r="H34" s="84"/>
-      <c r="I34" s="85"/>
+      <c r="G34" s="77"/>
+      <c r="H34" s="77"/>
+      <c r="I34" s="78"/>
     </row>
     <row r="35" spans="1:9" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A35" s="16" t="s">
@@ -2765,10 +2952,18 @@
       </c>
     </row>
     <row r="36" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A36" s="16"/>
-      <c r="B36" s="17"/>
-      <c r="C36" s="28"/>
-      <c r="D36" s="28"/>
+      <c r="A36" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="B36" s="17">
+        <v>6</v>
+      </c>
+      <c r="C36" s="28">
+        <v>5000</v>
+      </c>
+      <c r="D36" s="28">
+        <v>30000</v>
+      </c>
       <c r="E36" s="11"/>
       <c r="F36" s="17"/>
       <c r="G36" s="17"/>
@@ -2776,10 +2971,18 @@
       <c r="I36" s="28"/>
     </row>
     <row r="37" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A37" s="16"/>
-      <c r="B37" s="17"/>
-      <c r="C37" s="28"/>
-      <c r="D37" s="28"/>
+      <c r="A37" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B37" s="17">
+        <v>6</v>
+      </c>
+      <c r="C37" s="28">
+        <v>10000</v>
+      </c>
+      <c r="D37" s="28">
+        <v>60000</v>
+      </c>
       <c r="E37" s="11"/>
       <c r="F37" s="17"/>
       <c r="G37" s="17"/>
@@ -2787,10 +2990,18 @@
       <c r="I37" s="28"/>
     </row>
     <row r="38" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A38" s="16"/>
-      <c r="B38" s="17"/>
-      <c r="C38" s="28"/>
-      <c r="D38" s="28"/>
+      <c r="A38" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B38" s="17">
+        <v>6</v>
+      </c>
+      <c r="C38" s="28">
+        <v>5000</v>
+      </c>
+      <c r="D38" s="28">
+        <v>30000</v>
+      </c>
       <c r="E38" s="11"/>
       <c r="F38" s="17"/>
       <c r="G38" s="17"/>
@@ -2853,63 +3064,63 @@
       <c r="I43" s="28"/>
     </row>
     <row r="44" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A44" s="75" t="s">
+      <c r="A44" s="80" t="s">
         <v>9</v>
       </c>
-      <c r="B44" s="76"/>
-      <c r="C44" s="76"/>
+      <c r="B44" s="79"/>
+      <c r="C44" s="79"/>
       <c r="D44" s="28">
         <f>SUM(D36:D43)</f>
-        <v>0</v>
+        <v>120000</v>
       </c>
       <c r="E44" s="11"/>
-      <c r="F44" s="76" t="s">
+      <c r="F44" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="G44" s="76"/>
-      <c r="H44" s="76"/>
+      <c r="G44" s="79"/>
+      <c r="H44" s="79"/>
       <c r="I44" s="25">
         <f>SUM(I36:I43)</f>
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A45" s="75" t="s">
+      <c r="A45" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="B45" s="76"/>
-      <c r="C45" s="76"/>
+      <c r="B45" s="79"/>
+      <c r="C45" s="79"/>
       <c r="D45" s="28">
         <f>D44</f>
-        <v>0</v>
+        <v>120000</v>
       </c>
       <c r="E45" s="11"/>
-      <c r="F45" s="76" t="s">
+      <c r="F45" s="79" t="s">
         <v>10</v>
       </c>
-      <c r="G45" s="76"/>
-      <c r="H45" s="76"/>
+      <c r="G45" s="79"/>
+      <c r="H45" s="79"/>
       <c r="I45" s="25">
         <f>I44</f>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A46" s="75" t="s">
+      <c r="A46" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="B46" s="76"/>
-      <c r="C46" s="76"/>
+      <c r="B46" s="79"/>
+      <c r="C46" s="79"/>
       <c r="D46" s="28">
         <f>D44</f>
-        <v>0</v>
+        <v>120000</v>
       </c>
       <c r="E46" s="11"/>
-      <c r="F46" s="76" t="s">
+      <c r="F46" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="G46" s="76"/>
-      <c r="H46" s="76"/>
+      <c r="G46" s="79"/>
+      <c r="H46" s="79"/>
       <c r="I46" s="25">
         <f>I44</f>
         <v>0</v>
@@ -2941,11 +3152,11 @@
       <c r="A49" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="B49" s="80">
+      <c r="B49" s="66">
         <f>D32+I30+D44</f>
-        <v>0</v>
-      </c>
-      <c r="C49" s="80"/>
+        <v>1530000</v>
+      </c>
+      <c r="C49" s="66"/>
       <c r="D49" s="10"/>
       <c r="E49" s="11"/>
       <c r="F49" s="10"/>
@@ -2957,11 +3168,11 @@
       <c r="A50" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="B50" s="80">
+      <c r="B50" s="66">
         <f>D32+I30+D44</f>
-        <v>0</v>
-      </c>
-      <c r="C50" s="80"/>
+        <v>1530000</v>
+      </c>
+      <c r="C50" s="66"/>
       <c r="D50" s="10"/>
       <c r="E50" s="11"/>
       <c r="F50" s="11"/>
@@ -2973,8 +3184,8 @@
       <c r="A51" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="B51" s="66"/>
-      <c r="C51" s="66"/>
+      <c r="B51" s="94"/>
+      <c r="C51" s="94"/>
       <c r="D51" s="10"/>
       <c r="E51" s="11"/>
       <c r="F51" s="11"/>
@@ -2999,10 +3210,10 @@
       <c r="A53" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="B53" s="67" t="s">
+      <c r="B53" s="95" t="s">
         <v>18</v>
       </c>
-      <c r="C53" s="68"/>
+      <c r="C53" s="96"/>
       <c r="D53" s="10"/>
       <c r="E53" s="11"/>
       <c r="F53" s="11"/>
@@ -3011,14 +3222,14 @@
       <c r="I53" s="15"/>
     </row>
     <row r="54" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A54" s="20">
+      <c r="A54" s="20" t="str">
         <f>C6</f>
+        <v>JAVIER IGNACIO CAICEDO SAMBONI</v>
+      </c>
+      <c r="B54" s="97">
         <v>0</v>
       </c>
-      <c r="B54" s="69">
-        <v>0</v>
-      </c>
-      <c r="C54" s="70"/>
+      <c r="C54" s="98"/>
       <c r="D54" s="10"/>
       <c r="E54" s="11"/>
       <c r="F54" s="36"/>
@@ -3028,8 +3239,8 @@
     </row>
     <row r="55" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A55" s="40"/>
-      <c r="B55" s="69"/>
-      <c r="C55" s="70"/>
+      <c r="B55" s="97"/>
+      <c r="C55" s="98"/>
       <c r="D55" s="10"/>
       <c r="E55" s="11"/>
       <c r="F55" s="10"/>
@@ -3041,10 +3252,10 @@
       <c r="A56" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B56" s="71">
+      <c r="B56" s="99">
         <v>0</v>
       </c>
-      <c r="C56" s="72"/>
+      <c r="C56" s="100"/>
       <c r="D56" s="10"/>
       <c r="E56" s="11"/>
       <c r="F56" s="10"/>
@@ -3086,10 +3297,10 @@
       <c r="I59" s="44"/>
     </row>
     <row r="60" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A60" s="73" t="s">
+      <c r="A60" s="101" t="s">
         <v>20</v>
       </c>
-      <c r="B60" s="74"/>
+      <c r="B60" s="102"/>
       <c r="C60" s="11"/>
       <c r="D60" s="11"/>
       <c r="E60" s="11"/>
@@ -3104,31 +3315,35 @@
       <c r="A61" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="B61" s="61"/>
+      <c r="B61" s="61" t="s">
+        <v>57</v>
+      </c>
       <c r="C61" s="60"/>
       <c r="D61" s="11"/>
       <c r="E61" s="11"/>
       <c r="F61" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="G61" s="78"/>
-      <c r="H61" s="78"/>
-      <c r="I61" s="79"/>
+      <c r="G61" s="86"/>
+      <c r="H61" s="86"/>
+      <c r="I61" s="87"/>
     </row>
     <row r="62" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A62" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="B62" s="50"/>
+      <c r="B62" s="50">
+        <v>83040450</v>
+      </c>
       <c r="C62" s="11"/>
       <c r="D62" s="11"/>
       <c r="E62" s="11"/>
       <c r="F62" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="G62" s="86"/>
-      <c r="H62" s="86"/>
-      <c r="I62" s="87"/>
+      <c r="G62" s="64"/>
+      <c r="H62" s="64"/>
+      <c r="I62" s="65"/>
     </row>
     <row r="63" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A63" s="51"/>
@@ -3147,78 +3362,91 @@
       </c>
       <c r="B64" s="54"/>
       <c r="C64" s="11"/>
-      <c r="D64" s="62" t="s">
+      <c r="D64" s="90" t="s">
         <v>25</v>
       </c>
-      <c r="E64" s="62"/>
-      <c r="F64" s="62"/>
-      <c r="G64" s="62"/>
-      <c r="H64" s="62"/>
-      <c r="I64" s="63"/>
+      <c r="E64" s="90"/>
+      <c r="F64" s="90"/>
+      <c r="G64" s="90"/>
+      <c r="H64" s="90"/>
+      <c r="I64" s="91"/>
     </row>
     <row r="65" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A65" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="B65" s="21"/>
+      <c r="B65" s="21" t="s">
+        <v>58</v>
+      </c>
       <c r="C65" s="11"/>
-      <c r="D65" s="62"/>
-      <c r="E65" s="62"/>
-      <c r="F65" s="62"/>
-      <c r="G65" s="62"/>
-      <c r="H65" s="62"/>
-      <c r="I65" s="63"/>
+      <c r="D65" s="90"/>
+      <c r="E65" s="90"/>
+      <c r="F65" s="90"/>
+      <c r="G65" s="90"/>
+      <c r="H65" s="90"/>
+      <c r="I65" s="91"/>
     </row>
     <row r="66" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A66" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="B66" s="21"/>
+      <c r="B66" s="21" t="s">
+        <v>59</v>
+      </c>
       <c r="C66" s="11"/>
-      <c r="D66" s="62"/>
-      <c r="E66" s="62"/>
-      <c r="F66" s="62"/>
-      <c r="G66" s="62"/>
-      <c r="H66" s="62"/>
-      <c r="I66" s="63"/>
+      <c r="D66" s="90"/>
+      <c r="E66" s="90"/>
+      <c r="F66" s="90"/>
+      <c r="G66" s="90"/>
+      <c r="H66" s="90"/>
+      <c r="I66" s="91"/>
     </row>
     <row r="67" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A67" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="B67" s="21"/>
+      <c r="B67" s="21">
+        <v>86869831338</v>
+      </c>
       <c r="C67" s="11"/>
-      <c r="D67" s="62"/>
-      <c r="E67" s="62"/>
-      <c r="F67" s="62"/>
-      <c r="G67" s="62"/>
-      <c r="H67" s="62"/>
-      <c r="I67" s="63"/>
+      <c r="D67" s="90"/>
+      <c r="E67" s="90"/>
+      <c r="F67" s="90"/>
+      <c r="G67" s="90"/>
+      <c r="H67" s="90"/>
+      <c r="I67" s="91"/>
     </row>
     <row r="68" spans="1:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="B68" s="59"/>
+      <c r="B68" s="59" t="s">
+        <v>57</v>
+      </c>
       <c r="C68" s="56"/>
-      <c r="D68" s="64"/>
-      <c r="E68" s="64"/>
-      <c r="F68" s="64"/>
-      <c r="G68" s="64"/>
-      <c r="H68" s="64"/>
-      <c r="I68" s="65"/>
+      <c r="D68" s="92"/>
+      <c r="E68" s="92"/>
+      <c r="F68" s="92"/>
+      <c r="G68" s="92"/>
+      <c r="H68" s="92"/>
+      <c r="I68" s="93"/>
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="G62:I62"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="G61:I61"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="F45:H45"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="F32:H32"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="F34:I34"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="F44:H44"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="F30:H30"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="F31:H31"/>
     <mergeCell ref="D64:I68"/>
     <mergeCell ref="A1:I3"/>
     <mergeCell ref="A12:D12"/>
@@ -3235,20 +3463,15 @@
     <mergeCell ref="B49:C49"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="F30:H30"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="A45:C45"/>
-    <mergeCell ref="F45:H45"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="F32:H32"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="F34:I34"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="F44:H44"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="G62:I62"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="G61:I61"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3482,27 +3705,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="8962bb98-8ab0-4c0d-b40d-33b4d6a69b3f">YS7XHTTF5XVJ-1-44466</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="8962bb98-8ab0-4c0d-b40d-33b4d6a69b3f">
-      <Url>https://cmconsultores.sharepoint.com/sites/conectividad/_layouts/15/DocIdRedir.aspx?ID=YS7XHTTF5XVJ-1-44466</Url>
-      <Description>YS7XHTTF5XVJ-1-44466</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -3552,6 +3754,27 @@
 </spe:Receivers>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="8962bb98-8ab0-4c0d-b40d-33b4d6a69b3f">YS7XHTTF5XVJ-1-44466</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="8962bb98-8ab0-4c0d-b40d-33b4d6a69b3f">
+      <Url>https://cmconsultores.sharepoint.com/sites/conectividad/_layouts/15/DocIdRedir.aspx?ID=YS7XHTTF5XVJ-1-44466</Url>
+      <Description>YS7XHTTF5XVJ-1-44466</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8B8615D-B6A4-4F82-8F65-7B04E57B7446}">
   <ds:schemaRefs>
@@ -3572,18 +3795,9 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F6F7EAC-1687-4025-BE05-CDC3229FA3FF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{94ECD735-1F5C-4535-A9C4-4C3A61CAB4E8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="1984c043-b8ee-4b44-bc8d-2df04733c734"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="8962bb98-8ab0-4c0d-b40d-33b4d6a69b3f"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3597,9 +3811,18 @@
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{94ECD735-1F5C-4535-A9C4-4C3A61CAB4E8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F6F7EAC-1687-4025-BE05-CDC3229FA3FF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="1984c043-b8ee-4b44-bc8d-2df04733c734"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="8962bb98-8ab0-4c0d-b40d-33b4d6a69b3f"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>